<commit_message>
Resolved the Excel Issues
</commit_message>
<xml_diff>
--- a/REST/sample-xlsx-file.xlsx
+++ b/REST/sample-xlsx-file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nna15\GitHubProjects\math-board\REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01ACE05-43B6-4132-9EFB-B94CB6D51500}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D657105-E7C3-4A4B-9A9D-CB7351C7E98C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1775" yWindow="1775" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -28,54 +28,9 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Rajeev Singh</t>
-  </si>
-  <si>
-    <t>rajeev@example.com</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>john@example.com</t>
-  </si>
-  <si>
-    <t>Jack Sparrow</t>
-  </si>
-  <si>
-    <t>jack@example.com</t>
-  </si>
-  <si>
-    <t>Steven Cook</t>
-  </si>
-  <si>
-    <t>steven@example.com</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Teacher</t>
-  </si>
-  <si>
     <t>UserID</t>
   </si>
   <si>
@@ -85,20 +40,14 @@
     <t>Password</t>
   </si>
   <si>
-    <t>primary</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -106,12 +55,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -132,18 +75,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,17 +361,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -441,99 +380,36 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>5</v>
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
US56, Task75 - Session Handling for admin portal
</commit_message>
<xml_diff>
--- a/REST/sample-xlsx-file.xlsx
+++ b/REST/sample-xlsx-file.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nna15\GitHubProjects\math-board\REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D657105-E7C3-4A4B-9A9D-CB7351C7E98C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1D657105-E7C3-4A4B-9A9D-CB7351C7E98C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41"/>
   <bookViews>
-    <workbookView xWindow="1775" yWindow="1775" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="7380" windowWidth="14400" xWindow="1775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1775"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -41,12 +41,40 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>pwd*</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -76,17 +104,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -103,10 +131,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -141,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -176,7 +204,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -270,21 +298,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -301,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -353,23 +381,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.40625" defaultRowHeight="15.75" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row customHeight="1" ht="15.75" r="1" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -389,7 +417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.6">
+    <row ht="13" r="2" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -409,7 +437,67 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Expression Sheet to save expressions for session
</commit_message>
<xml_diff>
--- a/REST/sample-xlsx-file.xlsx
+++ b/REST/sample-xlsx-file.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nna15\GitHubProjects\math-board\REST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MS_Material\SER_515\Project_MathBoard\Git\math-board\REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D657105-E7C3-4A4B-9A9D-CB7351C7E98C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1775" yWindow="1775" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="14400" windowHeight="7380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Expression" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -41,12 +41,15 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>Expression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -360,16 +363,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -389,7 +392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -407,6 +410,29 @@
       </c>
       <c r="F2" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Sprint3 us11 save expression"
</commit_message>
<xml_diff>
--- a/REST/sample-xlsx-file.xlsx
+++ b/REST/sample-xlsx-file.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MS_Material\SER_515\Project_MathBoard\Git\math-board\REST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nna15\GitHubProjects\math-board\REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D657105-E7C3-4A4B-9A9D-CB7351C7E98C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="14400" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="1775" yWindow="1775" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
-    <sheet name="Expression" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -41,15 +41,12 @@
   </si>
   <si>
     <t>string</t>
-  </si>
-  <si>
-    <t>Expression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -363,16 +360,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -392,7 +389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -410,29 +407,6 @@
       </c>
       <c r="F2" t="s">
         <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
US_93: Quizzes storage to database
</commit_message>
<xml_diff>
--- a/REST/sample-xlsx-file.xlsx
+++ b/REST/sample-xlsx-file.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MS_Material\SER_515\Project_MathBoard\Git\math-board\REST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nna15\GitHubProjects\math-board\REST\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A37B64-D4E5-4E87-9262-5E49BC905D2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="14400" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
-    <sheet name="Expression" sheetId="2" r:id="rId2"/>
+    <sheet name="Quizzes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -43,13 +44,40 @@
     <t>string</t>
   </si>
   <si>
-    <t>Expression</t>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3+2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6+4</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>8+3</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -363,16 +391,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -392,7 +420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -418,21 +446,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A8" sqref="A8:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>